<commit_message>
started fixing MSNN increase
 - started fixing mainstem node number increase (WIP)
 - updated photoperiod filters in crops.xlsx
</commit_message>
<xml_diff>
--- a/input/crops.xlsx
+++ b/input/crops.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F5F07A-B02A-4B7C-B5ED-37863E307C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="0" windowWidth="35280" windowHeight="14660" activeTab="3"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wheat" sheetId="1" r:id="rId1"/>
@@ -12,8 +13,17 @@
     <sheet name="Maize" sheetId="4" r:id="rId3"/>
     <sheet name="allcrops" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -22,12 +32,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Auteur</author>
   </authors>
   <commentList>
-    <comment ref="A6" authorId="0">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -51,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -75,7 +85,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A19" authorId="0">
+    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -99,7 +109,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A68" authorId="0">
+    <comment ref="A68" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -128,12 +138,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Auteur</author>
   </authors>
   <commentList>
-    <comment ref="A6" authorId="0">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -157,7 +167,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -181,7 +191,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A19" authorId="0">
+    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -205,7 +215,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A70" authorId="0">
+    <comment ref="A70" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -234,12 +244,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Auteur</author>
   </authors>
   <commentList>
-    <comment ref="A22" authorId="0">
+    <comment ref="A22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -263,7 +273,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A23" authorId="0">
+    <comment ref="A23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -287,7 +297,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A24" authorId="0">
+    <comment ref="A24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -311,7 +321,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A33" authorId="0">
+    <comment ref="A33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -340,12 +350,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Auteur</author>
   </authors>
   <commentList>
-    <comment ref="A10" authorId="0">
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -369,7 +379,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0">
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -393,7 +403,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A24" authorId="0">
+    <comment ref="A24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -417,7 +427,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A55" authorId="0">
+    <comment ref="A55" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -441,7 +451,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A95" authorId="0">
+    <comment ref="A95" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
       <text>
         <r>
           <rPr>
@@ -465,7 +475,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A113" authorId="0">
+    <comment ref="A113" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
       <text>
         <r>
           <rPr>
@@ -489,7 +499,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P118" authorId="0">
+    <comment ref="P118" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000007000000}">
       <text>
         <r>
           <rPr>
@@ -1249,7 +1259,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -2071,13 +2081,16 @@
     <cellStyle name="Lien hypertexte visité" xfId="171" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="173" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-0000AD000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2369,23 +2382,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Feuil1" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="C68" sqref="C68:C76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="1" customWidth="1"/>
-    <col min="3" max="3" width="44.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="44.81640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2399,7 +2412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>97</v>
       </c>
@@ -2413,7 +2426,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>39</v>
       </c>
@@ -2427,7 +2440,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>40</v>
       </c>
@@ -2441,7 +2454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>41</v>
       </c>
@@ -2455,7 +2468,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>42</v>
       </c>
@@ -2467,7 +2480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>43</v>
       </c>
@@ -2479,7 +2492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>44</v>
       </c>
@@ -2493,7 +2506,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>45</v>
       </c>
@@ -2507,7 +2520,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>46</v>
       </c>
@@ -2521,7 +2534,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>47</v>
       </c>
@@ -2535,7 +2548,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>48</v>
       </c>
@@ -2547,7 +2560,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>49</v>
       </c>
@@ -2561,7 +2574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>50</v>
       </c>
@@ -2575,7 +2588,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
         <v>51</v>
       </c>
@@ -2589,7 +2602,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>52</v>
       </c>
@@ -2603,7 +2616,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>53</v>
       </c>
@@ -2617,7 +2630,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
         <v>54</v>
       </c>
@@ -2631,7 +2644,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>55</v>
       </c>
@@ -2643,7 +2656,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
         <v>56</v>
       </c>
@@ -2657,7 +2670,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
         <v>37</v>
       </c>
@@ -2671,7 +2684,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
         <v>57</v>
       </c>
@@ -2685,7 +2698,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
         <v>58</v>
       </c>
@@ -2699,7 +2712,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
         <v>59</v>
       </c>
@@ -2713,7 +2726,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
         <v>60</v>
       </c>
@@ -2727,7 +2740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
         <v>61</v>
       </c>
@@ -2741,7 +2754,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
         <v>62</v>
       </c>
@@ -2755,7 +2768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
         <v>63</v>
       </c>
@@ -2769,7 +2782,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
         <v>64</v>
       </c>
@@ -2783,7 +2796,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="12" t="s">
         <v>65</v>
       </c>
@@ -2797,7 +2810,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="8" t="s">
         <v>66</v>
       </c>
@@ -2811,7 +2824,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
         <v>67</v>
       </c>
@@ -2825,7 +2838,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="12" t="s">
         <v>68</v>
       </c>
@@ -2839,7 +2852,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="12" t="s">
         <v>69</v>
       </c>
@@ -2853,7 +2866,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="12" t="s">
         <v>70</v>
       </c>
@@ -2865,7 +2878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="12" t="s">
         <v>71</v>
       </c>
@@ -2879,7 +2892,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
         <v>72</v>
       </c>
@@ -2893,7 +2906,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
         <v>73</v>
       </c>
@@ -2907,7 +2920,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
         <v>74</v>
       </c>
@@ -2919,7 +2932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="12" t="s">
         <v>75</v>
       </c>
@@ -2933,7 +2946,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
         <v>76</v>
       </c>
@@ -2947,7 +2960,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="12" t="s">
         <v>77</v>
       </c>
@@ -2961,7 +2974,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="12" t="s">
         <v>78</v>
       </c>
@@ -2975,7 +2988,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="12" t="s">
         <v>38</v>
       </c>
@@ -2989,7 +3002,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="12" t="s">
         <v>79</v>
       </c>
@@ -3003,7 +3016,7 @@
         <v>2.0899999999999998E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="12" t="s">
         <v>80</v>
       </c>
@@ -3014,7 +3027,7 @@
         <v>2.0899999999999998E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="12" t="s">
         <v>81</v>
       </c>
@@ -3028,7 +3041,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="12" t="s">
         <v>82</v>
       </c>
@@ -3042,7 +3055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="12" t="s">
         <v>83</v>
       </c>
@@ -3056,7 +3069,7 @@
         <v>27.5</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="12" t="s">
         <v>84</v>
       </c>
@@ -3070,7 +3083,7 @@
         <v>27.5</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="12" t="s">
         <v>85</v>
       </c>
@@ -3084,7 +3097,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="12" t="s">
         <v>109</v>
       </c>
@@ -3096,7 +3109,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="12" t="s">
         <v>110</v>
       </c>
@@ -3107,7 +3120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="12" t="s">
         <v>111</v>
       </c>
@@ -3118,7 +3131,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="12" t="s">
         <v>112</v>
       </c>
@@ -3129,7 +3142,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="12" t="s">
         <v>113</v>
       </c>
@@ -3140,7 +3153,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="12" t="s">
         <v>86</v>
       </c>
@@ -3154,7 +3167,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="12" t="s">
         <v>87</v>
       </c>
@@ -3168,7 +3181,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="12" t="s">
         <v>88</v>
       </c>
@@ -3182,7 +3195,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="12" t="s">
         <v>23</v>
       </c>
@@ -3196,7 +3209,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="12" t="s">
         <v>25</v>
       </c>
@@ -3210,7 +3223,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="12" t="s">
         <v>26</v>
       </c>
@@ -3224,7 +3237,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="12" t="s">
         <v>27</v>
       </c>
@@ -3238,7 +3251,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="12" t="s">
         <v>28</v>
       </c>
@@ -3252,7 +3265,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="12" t="s">
         <v>29</v>
       </c>
@@ -3266,7 +3279,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="12" t="s">
         <v>30</v>
       </c>
@@ -3280,7 +3293,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="12" t="s">
         <v>31</v>
       </c>
@@ -3294,7 +3307,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:5" s="1" customFormat="1">
+    <row r="68" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="32" t="s">
         <v>98</v>
       </c>
@@ -3309,7 +3322,7 @@
       </c>
       <c r="E68" s="30"/>
     </row>
-    <row r="69" spans="1:5" s="1" customFormat="1">
+    <row r="69" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69" s="34" t="s">
         <v>99</v>
       </c>
@@ -3322,7 +3335,7 @@
       </c>
       <c r="E69" s="30"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="35" t="s">
         <v>100</v>
       </c>
@@ -3335,7 +3348,7 @@
       </c>
       <c r="E70" s="31"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="32" t="s">
         <v>101</v>
       </c>
@@ -3348,7 +3361,7 @@
       </c>
       <c r="E71" s="31"/>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="32" t="s">
         <v>102</v>
       </c>
@@ -3361,7 +3374,7 @@
       </c>
       <c r="E72" s="31"/>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="32" t="s">
         <v>103</v>
       </c>
@@ -3374,22 +3387,22 @@
       </c>
       <c r="E73" s="31"/>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="32" t="s">
         <v>104</v>
       </c>
       <c r="B74" s="32"/>
       <c r="C74" s="33" t="str">
         <f>"is.after('anthesis', 5) &amp; is.before('anthesis', "&amp; C66-1.5 &amp; ")"</f>
-        <v>is.after('anthesis', 5) &amp; is.before('anthesis', 41.5)</v>
+        <v>is.after('anthesis', 5) &amp; is.before('anthesis', 41,5)</v>
       </c>
       <c r="D74" s="33" t="str">
         <f>"is.after('anthesis', 5) &amp; is.before('anthesis', "&amp; D66-1.5 &amp; ")"</f>
-        <v>is.after('anthesis', 5) &amp; is.before('anthesis', 41.5)</v>
+        <v>is.after('anthesis', 5) &amp; is.before('anthesis', 41,5)</v>
       </c>
       <c r="E74" s="31"/>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="35" t="s">
         <v>105</v>
       </c>
@@ -3400,11 +3413,11 @@
       </c>
       <c r="D75" s="33" t="str">
         <f>"is.after('germination') &amp; is.before('anthesis', "&amp; D66-1.5 &amp;")"</f>
-        <v>is.after('germination') &amp; is.before('anthesis', 41.5)</v>
+        <v>is.after('germination') &amp; is.before('anthesis', 41,5)</v>
       </c>
       <c r="E75" s="31"/>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>114</v>
       </c>
@@ -3416,7 +3429,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B77" s="14"/>
       <c r="C77"/>
       <c r="D77"/>
@@ -3435,17 +3448,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Feuil2" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:C79"/>
   <sheetViews>
     <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="A57" sqref="A57:A62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3456,7 +3469,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>97</v>
       </c>
@@ -3467,7 +3480,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>39</v>
       </c>
@@ -3476,7 +3489,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>40</v>
       </c>
@@ -3485,7 +3498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>41</v>
       </c>
@@ -3494,7 +3507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>42</v>
       </c>
@@ -3503,7 +3516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>43</v>
       </c>
@@ -3512,7 +3525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>44</v>
       </c>
@@ -3521,7 +3534,7 @@
         <v>1.61E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>45</v>
       </c>
@@ -3530,7 +3543,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>46</v>
       </c>
@@ -3539,7 +3552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>47</v>
       </c>
@@ -3548,7 +3561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>48</v>
       </c>
@@ -3557,7 +3570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>49</v>
       </c>
@@ -3566,7 +3579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>50</v>
       </c>
@@ -3575,7 +3588,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
         <v>51</v>
       </c>
@@ -3584,7 +3597,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>52</v>
       </c>
@@ -3593,7 +3606,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>53</v>
       </c>
@@ -3602,7 +3615,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
         <v>54</v>
       </c>
@@ -3611,7 +3624,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>55</v>
       </c>
@@ -3620,7 +3633,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
         <v>56</v>
       </c>
@@ -3629,7 +3642,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
         <v>37</v>
       </c>
@@ -3638,7 +3651,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
         <v>57</v>
       </c>
@@ -3647,7 +3660,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
         <v>58</v>
       </c>
@@ -3656,7 +3669,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
         <v>59</v>
       </c>
@@ -3665,7 +3678,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
         <v>60</v>
       </c>
@@ -3674,7 +3687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
         <v>61</v>
       </c>
@@ -3683,7 +3696,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
         <v>62</v>
       </c>
@@ -3692,7 +3705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
         <v>63</v>
       </c>
@@ -3701,7 +3714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
         <v>64</v>
       </c>
@@ -3710,7 +3723,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="12" t="s">
         <v>65</v>
       </c>
@@ -3719,7 +3732,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="8" t="s">
         <v>66</v>
       </c>
@@ -3728,7 +3741,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="8" t="s">
         <v>67</v>
       </c>
@@ -3737,7 +3750,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="8" t="s">
         <v>68</v>
       </c>
@@ -3746,7 +3759,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="13" t="s">
         <v>69</v>
       </c>
@@ -3755,7 +3768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="13" t="s">
         <v>70</v>
       </c>
@@ -3764,7 +3777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="8" t="s">
         <v>71</v>
       </c>
@@ -3773,7 +3786,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="8" t="s">
         <v>72</v>
       </c>
@@ -3782,7 +3795,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="8" t="s">
         <v>73</v>
       </c>
@@ -3791,7 +3804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="8" t="s">
         <v>74</v>
       </c>
@@ -3800,7 +3813,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="12" t="s">
         <v>75</v>
       </c>
@@ -3809,7 +3822,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="8" t="s">
         <v>76</v>
       </c>
@@ -3818,7 +3831,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="8" t="s">
         <v>77</v>
       </c>
@@ -3827,7 +3840,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="8" t="s">
         <v>78</v>
       </c>
@@ -3836,7 +3849,7 @@
         <v>1.37E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="8" t="s">
         <v>38</v>
       </c>
@@ -3845,7 +3858,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="8" t="s">
         <v>79</v>
       </c>
@@ -3854,7 +3867,7 @@
         <v>3.3700000000000001E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="8" t="s">
         <v>80</v>
       </c>
@@ -3863,7 +3876,7 @@
         <v>3.3700000000000001E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="8" t="s">
         <v>81</v>
       </c>
@@ -3872,7 +3885,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="8" t="s">
         <v>82</v>
       </c>
@@ -3881,7 +3894,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="8" t="s">
         <v>83</v>
       </c>
@@ -3890,7 +3903,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="8" t="s">
         <v>84</v>
       </c>
@@ -3899,7 +3912,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="8" t="s">
         <v>85</v>
       </c>
@@ -3908,7 +3921,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="8" t="s">
         <v>86</v>
       </c>
@@ -3918,7 +3931,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="8" t="s">
         <v>87</v>
       </c>
@@ -3927,7 +3940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="8" t="s">
         <v>88</v>
       </c>
@@ -3936,7 +3949,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="16" t="s">
         <v>23</v>
       </c>
@@ -3945,7 +3958,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="17" t="s">
         <v>25</v>
       </c>
@@ -3954,7 +3967,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="17" t="s">
         <v>26</v>
       </c>
@@ -3963,7 +3976,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="17" t="s">
         <v>27</v>
       </c>
@@ -3972,7 +3985,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="17" t="s">
         <v>28</v>
       </c>
@@ -3981,7 +3994,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="17" t="s">
         <v>29</v>
       </c>
@@ -3990,7 +4003,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="17" t="s">
         <v>30</v>
       </c>
@@ -3999,7 +4012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="17" t="s">
         <v>31</v>
       </c>
@@ -4008,7 +4021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="18" t="s">
         <v>89</v>
       </c>
@@ -4017,7 +4030,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="19" t="s">
         <v>90</v>
       </c>
@@ -4026,7 +4039,7 @@
         <v>76.5</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="20" t="s">
         <v>91</v>
       </c>
@@ -4035,7 +4048,7 @@
         <v>54.5</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="20" t="s">
         <v>92</v>
       </c>
@@ -4044,7 +4057,7 @@
         <v>76.5</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="18" t="s">
         <v>93</v>
       </c>
@@ -4053,7 +4066,7 @@
         <v>52.5</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="18" t="s">
         <v>94</v>
       </c>
@@ -4062,7 +4075,7 @@
         <v>60.1</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="18" t="s">
         <v>95</v>
       </c>
@@ -4071,7 +4084,7 @@
         <v>54.5</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="21" t="s">
         <v>96</v>
       </c>
@@ -4080,16 +4093,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="32" t="s">
         <v>98</v>
       </c>
       <c r="C71" t="str">
         <f>"list(germination= "&amp; C63 &amp;", vegetativegrowth=" &amp;C65&amp;" ,reproductivegrowth="&amp;C66&amp;")"</f>
-        <v>list(germination= 8.5, vegetativegrowth=54.5 ,reproductivegrowth=76.5)</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
+        <v>list(germination= 8,5, vegetativegrowth=54,5 ,reproductivegrowth=76,5)</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="34" t="s">
         <v>99</v>
       </c>
@@ -4097,7 +4110,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="35" t="s">
         <v>100</v>
       </c>
@@ -4105,7 +4118,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="32" t="s">
         <v>101</v>
       </c>
@@ -4113,7 +4126,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="32" t="s">
         <v>102</v>
       </c>
@@ -4121,7 +4134,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="32" t="s">
         <v>103</v>
       </c>
@@ -4129,7 +4142,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="32" t="s">
         <v>104</v>
       </c>
@@ -4137,7 +4150,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="35" t="s">
         <v>105</v>
       </c>
@@ -4145,7 +4158,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>114</v>
       </c>
@@ -4166,16 +4179,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="70">
         <v>1</v>
       </c>
@@ -4186,13 +4199,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="40" t="s">
         <v>119</v>
       </c>
@@ -4201,7 +4214,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -4210,7 +4223,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>120</v>
       </c>
@@ -4219,7 +4232,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="74" t="s">
         <v>171</v>
       </c>
@@ -4230,7 +4243,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="74" t="s">
         <v>172</v>
       </c>
@@ -4241,7 +4254,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="74" t="s">
         <v>173</v>
       </c>
@@ -4252,7 +4265,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="74" t="s">
         <v>174</v>
       </c>
@@ -4263,47 +4276,47 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="74"/>
       <c r="B11" s="9"/>
       <c r="C11" s="67"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="74"/>
       <c r="B12" s="9"/>
       <c r="C12" s="67"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="74"/>
       <c r="B13" s="9"/>
       <c r="C13" s="67"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="74"/>
       <c r="B14" s="9"/>
       <c r="C14" s="67"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="74"/>
       <c r="B15" s="9"/>
       <c r="C15" s="67"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="74"/>
       <c r="B16" s="9"/>
       <c r="C16" s="67"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="74"/>
       <c r="B17" s="9"/>
       <c r="C17" s="67"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="74"/>
       <c r="B18" s="9"/>
       <c r="C18" s="67"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="74" t="s">
         <v>176</v>
       </c>
@@ -4314,7 +4327,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="74" t="s">
         <v>177</v>
       </c>
@@ -4325,12 +4338,12 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="75"/>
       <c r="B21" s="51"/>
       <c r="C21" s="68"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="76" t="s">
         <v>23</v>
       </c>
@@ -4341,7 +4354,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="76" t="s">
         <v>223</v>
       </c>
@@ -4352,7 +4365,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="76" t="s">
         <v>224</v>
       </c>
@@ -4363,37 +4376,37 @@
         <v>33.799999999999997</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="76"/>
       <c r="B25" s="9"/>
       <c r="C25" s="68"/>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="76"/>
       <c r="B26" s="9"/>
       <c r="C26" s="68"/>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="76"/>
       <c r="B27" s="9"/>
       <c r="C27" s="68"/>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="76"/>
       <c r="B28" s="9"/>
       <c r="C28" s="69"/>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="76"/>
       <c r="B29" s="9"/>
       <c r="C29" s="68"/>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="75"/>
       <c r="B30" s="51"/>
       <c r="C30" s="68"/>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="75" t="s">
         <v>126</v>
       </c>
@@ -4404,7 +4417,7 @@
         <v>38.9</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="74" t="s">
         <v>127</v>
       </c>
@@ -4415,7 +4428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="75" t="s">
         <v>225</v>
       </c>
@@ -4424,7 +4437,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="75" t="s">
         <v>131</v>
       </c>
@@ -4435,7 +4448,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="74" t="s">
         <v>226</v>
       </c>
@@ -4446,7 +4459,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="77" t="s">
         <v>227</v>
       </c>
@@ -4457,12 +4470,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="75"/>
       <c r="B37" s="11"/>
       <c r="C37" s="78"/>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="74" t="s">
         <v>136</v>
       </c>
@@ -4473,7 +4486,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="74" t="s">
         <v>137</v>
       </c>
@@ -4484,7 +4497,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="74" t="s">
         <v>138</v>
       </c>
@@ -4495,7 +4508,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="74" t="s">
         <v>139</v>
       </c>
@@ -4506,7 +4519,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="75" t="s">
         <v>140</v>
       </c>
@@ -4517,7 +4530,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="75" t="s">
         <v>141</v>
       </c>
@@ -4528,12 +4541,12 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="75"/>
       <c r="B44" s="9"/>
       <c r="C44" s="66"/>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="75" t="s">
         <v>143</v>
       </c>
@@ -4544,7 +4557,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="75" t="s">
         <v>144</v>
       </c>
@@ -4555,7 +4568,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="75" t="s">
         <v>145</v>
       </c>
@@ -4566,7 +4579,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="75" t="s">
         <v>146</v>
       </c>
@@ -4577,7 +4590,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="75" t="s">
         <v>147</v>
       </c>
@@ -4588,7 +4601,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="74" t="s">
         <v>148</v>
       </c>
@@ -4599,7 +4612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="76" t="s">
         <v>149</v>
       </c>
@@ -4610,7 +4623,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="77" t="s">
         <v>150</v>
       </c>
@@ -4621,7 +4634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="77" t="s">
         <v>151</v>
       </c>
@@ -4632,7 +4645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="77" t="s">
         <v>152</v>
       </c>
@@ -4643,7 +4656,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="77" t="s">
         <v>153</v>
       </c>
@@ -4654,12 +4667,12 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="75"/>
       <c r="B56" s="9"/>
       <c r="C56" s="66"/>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="74" t="s">
         <v>154</v>
       </c>
@@ -4670,7 +4683,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="75" t="s">
         <v>155</v>
       </c>
@@ -4681,7 +4694,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="74" t="s">
         <v>156</v>
       </c>
@@ -4692,7 +4705,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="74" t="s">
         <v>228</v>
       </c>
@@ -4703,7 +4716,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="74" t="s">
         <v>159</v>
       </c>
@@ -4714,7 +4727,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="74" t="s">
         <v>160</v>
       </c>
@@ -4725,7 +4738,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="74" t="s">
         <v>161</v>
       </c>
@@ -4736,7 +4749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="77" t="s">
         <v>163</v>
       </c>
@@ -4747,12 +4760,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="75"/>
       <c r="B65" s="9"/>
       <c r="C65" s="66"/>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="75" t="s">
         <v>164</v>
       </c>
@@ -4763,7 +4776,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="75" t="s">
         <v>165</v>
       </c>
@@ -4774,7 +4787,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="75" t="s">
         <v>166</v>
       </c>
@@ -4785,7 +4798,7 @@
         <v>1.06E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="75" t="s">
         <v>167</v>
       </c>
@@ -4796,7 +4809,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="75" t="s">
         <v>229</v>
       </c>
@@ -4807,7 +4820,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="75" t="s">
         <v>170</v>
       </c>
@@ -4818,7 +4831,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="75"/>
       <c r="B72" s="9"/>
       <c r="C72" s="66"/>
@@ -4835,32 +4848,32 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Feuil3" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Feuil3"/>
   <dimension ref="A1:P120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B91" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B87" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="J120" sqref="J120"/>
+      <selection pane="bottomRight" activeCell="L101" sqref="L101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="8" max="8" width="17.1640625" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" customWidth="1"/>
-    <col min="12" max="12" width="16.1640625" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" customWidth="1"/>
-    <col min="15" max="15" width="36.6640625" customWidth="1"/>
-    <col min="16" max="16" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.1796875" customWidth="1"/>
+    <col min="4" max="4" width="21.6328125" customWidth="1"/>
+    <col min="5" max="5" width="8.6328125" customWidth="1"/>
+    <col min="8" max="8" width="17.1796875" customWidth="1"/>
+    <col min="10" max="10" width="12.6328125" customWidth="1"/>
+    <col min="12" max="12" width="16.1796875" customWidth="1"/>
+    <col min="14" max="14" width="11.6328125" customWidth="1"/>
+    <col min="15" max="15" width="36.6328125" customWidth="1"/>
+    <col min="16" max="16" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" hidden="1">
+    <row r="1" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A1" s="37"/>
       <c r="B1" s="37"/>
       <c r="C1" s="38"/>
@@ -4876,7 +4889,7 @@
       <c r="M1" s="37"/>
       <c r="N1" s="37"/>
     </row>
-    <row r="2" spans="1:16" hidden="1">
+    <row r="2" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
       <c r="D2" s="2"/>
       <c r="F2" s="1"/>
@@ -4889,7 +4902,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:16" hidden="1">
+    <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
       <c r="D3" s="37">
         <v>3</v>
@@ -4914,7 +4927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="40" t="s">
         <v>119</v>
       </c>
@@ -4949,7 +4962,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -4976,7 +4989,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>120</v>
       </c>
@@ -5007,7 +5020,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>126</v>
       </c>
@@ -5036,7 +5049,7 @@
         <v>38.9</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>127</v>
       </c>
@@ -5065,7 +5078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>128</v>
       </c>
@@ -5094,7 +5107,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>129</v>
       </c>
@@ -5118,7 +5131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>130</v>
       </c>
@@ -5142,7 +5155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>131</v>
       </c>
@@ -5171,7 +5184,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>132</v>
       </c>
@@ -5200,7 +5213,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>133</v>
       </c>
@@ -5229,7 +5242,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
         <v>134</v>
       </c>
@@ -5255,7 +5268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>135</v>
       </c>
@@ -5279,7 +5292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="8"/>
       <c r="B17" s="9"/>
       <c r="D17" s="10"/>
@@ -5289,7 +5302,7 @@
       <c r="L17" s="10"/>
       <c r="N17" s="10"/>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
         <v>136</v>
       </c>
@@ -5318,7 +5331,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>137</v>
       </c>
@@ -5347,7 +5360,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
         <v>138</v>
       </c>
@@ -5376,7 +5389,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
         <v>139</v>
       </c>
@@ -5405,7 +5418,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
         <v>140</v>
       </c>
@@ -5434,7 +5447,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
         <v>141</v>
       </c>
@@ -5463,7 +5476,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
         <v>142</v>
       </c>
@@ -5487,7 +5500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="12"/>
       <c r="B25" s="9"/>
       <c r="D25" s="10"/>
@@ -5497,7 +5510,7 @@
       <c r="L25" s="10"/>
       <c r="N25" s="10"/>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
         <v>143</v>
       </c>
@@ -5526,7 +5539,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
         <v>144</v>
       </c>
@@ -5555,7 +5568,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
         <v>145</v>
       </c>
@@ -5584,7 +5597,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="8" t="s">
         <v>146</v>
       </c>
@@ -5613,7 +5626,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
         <v>147</v>
       </c>
@@ -5642,7 +5655,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="8" t="s">
         <v>148</v>
       </c>
@@ -5671,7 +5684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
         <v>149</v>
       </c>
@@ -5700,7 +5713,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" s="12" t="s">
         <v>150</v>
       </c>
@@ -5729,7 +5742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" s="12" t="s">
         <v>151</v>
       </c>
@@ -5758,7 +5771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" s="12" t="s">
         <v>152</v>
       </c>
@@ -5787,7 +5800,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" s="12" t="s">
         <v>153</v>
       </c>
@@ -5816,7 +5829,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" s="43"/>
       <c r="B37" s="44"/>
       <c r="C37" s="45"/>
@@ -5828,7 +5841,7 @@
       <c r="L37" s="10"/>
       <c r="N37" s="10"/>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" s="43"/>
       <c r="B38" s="9"/>
       <c r="D38" s="10"/>
@@ -5838,7 +5851,7 @@
       <c r="L38" s="10"/>
       <c r="N38" s="10"/>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" s="43"/>
       <c r="B39" s="9"/>
       <c r="D39" s="10"/>
@@ -5848,7 +5861,7 @@
       <c r="L39" s="10"/>
       <c r="N39" s="10"/>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" s="47"/>
       <c r="B40" s="9"/>
       <c r="D40" s="10"/>
@@ -5858,7 +5871,7 @@
       <c r="L40" s="10"/>
       <c r="N40" s="10"/>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" s="43"/>
       <c r="B41" s="11"/>
       <c r="D41" s="10"/>
@@ -5868,7 +5881,7 @@
       <c r="L41" s="10"/>
       <c r="N41" s="10"/>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" s="43"/>
       <c r="B42" s="9"/>
       <c r="D42" s="10"/>
@@ -5878,7 +5891,7 @@
       <c r="L42" s="10"/>
       <c r="N42" s="10"/>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" s="43"/>
       <c r="B43" s="9"/>
       <c r="D43" s="10"/>
@@ -5888,7 +5901,7 @@
       <c r="L43" s="10"/>
       <c r="N43" s="10"/>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" s="8"/>
       <c r="B44" s="9"/>
       <c r="D44" s="10"/>
@@ -5898,7 +5911,7 @@
       <c r="L44" s="10"/>
       <c r="N44" s="10"/>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" s="8" t="s">
         <v>154</v>
       </c>
@@ -5927,7 +5940,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" s="8" t="s">
         <v>155</v>
       </c>
@@ -5956,7 +5969,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47" s="8" t="s">
         <v>156</v>
       </c>
@@ -5985,7 +5998,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:16">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" s="13" t="s">
         <v>157</v>
       </c>
@@ -6014,7 +6027,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A49" s="13" t="s">
         <v>158</v>
       </c>
@@ -6038,7 +6051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50" s="8" t="s">
         <v>159</v>
       </c>
@@ -6067,7 +6080,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51" s="8" t="s">
         <v>160</v>
       </c>
@@ -6096,7 +6109,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A52" s="8" t="s">
         <v>161</v>
       </c>
@@ -6125,7 +6138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A53" s="8" t="s">
         <v>162</v>
       </c>
@@ -6149,7 +6162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A54" s="12" t="s">
         <v>163</v>
       </c>
@@ -6178,7 +6191,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A55" s="64"/>
       <c r="B55" s="9"/>
       <c r="D55" s="10"/>
@@ -6188,7 +6201,7 @@
       <c r="L55" s="63"/>
       <c r="N55" s="63"/>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A56" s="64"/>
       <c r="B56" s="1"/>
       <c r="D56" s="10"/>
@@ -6198,7 +6211,7 @@
       <c r="L56" s="63"/>
       <c r="N56" s="63"/>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A57" s="64"/>
       <c r="B57" s="1"/>
       <c r="D57" s="10"/>
@@ -6208,7 +6221,7 @@
       <c r="L57" s="63"/>
       <c r="N57" s="63"/>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A58" s="64"/>
       <c r="B58" s="1"/>
       <c r="D58" s="10"/>
@@ -6218,7 +6231,7 @@
       <c r="L58" s="63"/>
       <c r="N58" s="63"/>
     </row>
-    <row r="59" spans="1:16">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59" s="64"/>
       <c r="B59" s="1"/>
       <c r="D59" s="10"/>
@@ -6228,7 +6241,7 @@
       <c r="L59" s="63"/>
       <c r="N59" s="63"/>
     </row>
-    <row r="60" spans="1:16">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A60" s="47"/>
       <c r="B60" s="9"/>
       <c r="D60" s="15"/>
@@ -6238,7 +6251,7 @@
       <c r="L60" s="15"/>
       <c r="N60" s="15"/>
     </row>
-    <row r="61" spans="1:16">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A61" s="8" t="s">
         <v>164</v>
       </c>
@@ -6267,7 +6280,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A62" s="8" t="s">
         <v>165</v>
       </c>
@@ -6296,7 +6309,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="63" spans="1:16">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A63" s="8" t="s">
         <v>166</v>
       </c>
@@ -6325,7 +6338,7 @@
         <v>1.06E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A64" s="8" t="s">
         <v>167</v>
       </c>
@@ -6354,7 +6367,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:16">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" s="8" t="s">
         <v>168</v>
       </c>
@@ -6383,7 +6396,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:16">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" s="8" t="s">
         <v>169</v>
       </c>
@@ -6410,7 +6423,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="67" spans="1:16">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67" s="8" t="s">
         <v>170</v>
       </c>
@@ -6436,7 +6449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68" s="8"/>
       <c r="B68" s="9"/>
       <c r="D68" s="10"/>
@@ -6446,7 +6459,7 @@
       <c r="L68" s="10"/>
       <c r="N68" s="10"/>
     </row>
-    <row r="69" spans="1:16">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" s="8" t="s">
         <v>171</v>
       </c>
@@ -6475,7 +6488,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:16">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" s="8" t="s">
         <v>172</v>
       </c>
@@ -6504,7 +6517,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="1:16">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" s="8" t="s">
         <v>173</v>
       </c>
@@ -6533,7 +6546,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:16">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A72" s="8" t="s">
         <v>174</v>
       </c>
@@ -6562,7 +6575,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="73" spans="1:16">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73" s="50"/>
       <c r="B73" s="9"/>
       <c r="D73" s="48"/>
@@ -6572,7 +6585,7 @@
       <c r="L73" s="48"/>
       <c r="N73" s="48"/>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A74" s="8" t="s">
         <v>175</v>
       </c>
@@ -6598,7 +6611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:16">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A75" s="8"/>
       <c r="B75" s="9"/>
       <c r="D75" s="10"/>
@@ -6608,7 +6621,7 @@
       <c r="L75" s="10"/>
       <c r="N75" s="10"/>
     </row>
-    <row r="76" spans="1:16">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A76" s="8" t="s">
         <v>176</v>
       </c>
@@ -6637,7 +6650,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="77" spans="1:16">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A77" s="8" t="s">
         <v>177</v>
       </c>
@@ -6666,7 +6679,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="78" spans="1:16">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A78" s="8"/>
       <c r="B78" s="51"/>
       <c r="D78" s="10"/>
@@ -6676,7 +6689,7 @@
       <c r="L78" s="10"/>
       <c r="N78" s="10"/>
     </row>
-    <row r="79" spans="1:16">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A79" s="16" t="s">
         <v>23</v>
       </c>
@@ -6705,7 +6718,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:16">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A80" s="17" t="s">
         <v>25</v>
       </c>
@@ -6734,7 +6747,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="81" spans="1:16">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A81" s="17" t="s">
         <v>26</v>
       </c>
@@ -6763,7 +6776,7 @@
         <v>33.799999999999997</v>
       </c>
     </row>
-    <row r="82" spans="1:16">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A82" s="17" t="s">
         <v>27</v>
       </c>
@@ -6789,7 +6802,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:16">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A83" s="17" t="s">
         <v>28</v>
       </c>
@@ -6815,7 +6828,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:16">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A84" s="17" t="s">
         <v>29</v>
       </c>
@@ -6841,7 +6854,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:16">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A85" s="17" t="s">
         <v>30</v>
       </c>
@@ -6867,7 +6880,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="86" spans="1:16">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A86" s="17" t="s">
         <v>31</v>
       </c>
@@ -6893,7 +6906,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:16">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
       <c r="E87" s="1"/>
       <c r="F87" s="39"/>
       <c r="H87" s="39"/>
@@ -6901,7 +6914,7 @@
       <c r="L87" s="39"/>
       <c r="N87" s="39"/>
     </row>
-    <row r="88" spans="1:16">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A88" s="18" t="s">
         <v>178</v>
       </c>
@@ -6929,7 +6942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:16">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A89" s="19" t="s">
         <v>179</v>
       </c>
@@ -6957,7 +6970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:16">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A90" s="20" t="s">
         <v>180</v>
       </c>
@@ -6983,7 +6996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:16">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A91" s="20" t="s">
         <v>181</v>
       </c>
@@ -7009,7 +7022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:16">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A92" s="18" t="s">
         <v>182</v>
       </c>
@@ -7037,7 +7050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:16">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A93" s="18" t="s">
         <v>183</v>
       </c>
@@ -7065,7 +7078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:16">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A94" s="18" t="s">
         <v>184</v>
       </c>
@@ -7093,7 +7106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:16">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A95" s="21" t="s">
         <v>185</v>
       </c>
@@ -7122,7 +7135,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="96" spans="1:16">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A96" s="59" t="s">
         <v>98</v>
       </c>
@@ -7132,27 +7145,27 @@
       <c r="C96" s="1"/>
       <c r="D96" s="65" t="str">
         <f>"c(germination="&amp;D79&amp;",leafDevelopment="&amp;D80&amp;",tillering="&amp;D81&amp;",stemElongation="&amp;D82&amp;",booting="&amp;D83&amp;",earing="&amp;D84&amp;",anthesis=5,  grainFilling="&amp;D85-5-1.5&amp;", maturation=1.5, senescence="&amp;D86&amp;", harvested=Inf)"</f>
-        <v>c(germination=6,leafDevelopment=5,tillering=8,stemElongation=6,booting=6,earing=15,anthesis=5,  grainFilling=36.5, maturation=1.5, senescence=8, harvested=Inf)</v>
+        <v>c(germination=6,leafDevelopment=5,tillering=8,stemElongation=6,booting=6,earing=15,anthesis=5,  grainFilling=36,5, maturation=1.5, senescence=8, harvested=Inf)</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="33" t="str">
         <f>"c(germination="&amp;F79&amp;",leafDevelopment="&amp;F80&amp;",tillering="&amp;F81&amp;",stemElongation="&amp;F82&amp;",booting="&amp;F83&amp;",earing="&amp;F84&amp;",anthesis=5,  grainFilling="&amp;F85-5-1.5&amp;", maturation=1.5, senescence="&amp;F86&amp;", harvested=Inf)"</f>
-        <v>c(germination=4,leafDevelopment=9.49254658375,tillering=7.77406832435,stemElongation=2.58226465555556,booting=0.645568438888889,earing=3.15555555555556,anthesis=5,  grainFilling=33.9, maturation=1.5, senescence=8, harvested=Inf)</v>
+        <v>c(germination=4,leafDevelopment=9,49254658375,tillering=7,77406832435,stemElongation=2,58226465555556,booting=0,645568438888889,earing=3,15555555555556,anthesis=5,  grainFilling=33,9, maturation=1.5, senescence=8, harvested=Inf)</v>
       </c>
       <c r="G96" s="56"/>
       <c r="H96" s="33" t="str">
         <f>"c(germination="&amp;H79&amp;",leafDevelopment="&amp;H80&amp;",tillering="&amp;H81&amp;",stemElongation="&amp;H82&amp;",booting="&amp;H83&amp;",earing="&amp;H84&amp;",anthesis=5,  grainFilling="&amp;H85-5-1.5&amp;", maturation=1.5, senescence="&amp;H86&amp;", harvested=Inf)"</f>
-        <v>c(germination=4,leafDevelopment=11.6,tillering=9.5,stemElongation=3.15555555555556,booting=0.788888888888889,earing=3.15555555555556,anthesis=5,  grainFilling=31.1, maturation=1.5, senescence=8, harvested=Inf)</v>
+        <v>c(germination=4,leafDevelopment=11,6,tillering=9,5,stemElongation=3,15555555555556,booting=0,788888888888889,earing=3,15555555555556,anthesis=5,  grainFilling=31,1, maturation=1.5, senescence=8, harvested=Inf)</v>
       </c>
       <c r="I96" s="56"/>
       <c r="J96" s="33" t="str">
         <f>"c(SOW="&amp;J79&amp;" ,EMR="&amp;J80&amp;", R1="&amp;J81&amp;", R3="&amp;J82&amp;", R5="&amp;J83&amp;", R7="&amp;J84&amp;", R8=Inf)"</f>
-        <v>c(SOW=8.5 ,EMR=36, R1=5.7, R3=4.3, R5=22, R7=7, R8=Inf)</v>
+        <v>c(SOW=8,5 ,EMR=36, R1=5,7, R3=4,3, R5=22, R7=7, R8=Inf)</v>
       </c>
       <c r="K96" s="56"/>
       <c r="L96" s="33" t="str">
         <f>"c(germination="&amp;L79&amp;",leafDevelopment="&amp;L80&amp;",tillering="&amp;L81&amp;",stemElongation="&amp;L82&amp;",booting="&amp;L83&amp;",earing="&amp;L84&amp;",anthesis=5,  grainFilling="&amp;L85-5-1.5&amp;", maturation=1.5, senescence="&amp;L86&amp;", harvested=Inf)"</f>
-        <v>c(germination=0,leafDevelopment=0,tillering=0,stemElongation=0,booting=0,earing=0,anthesis=5,  grainFilling=-6.5, maturation=1.5, senescence=0, harvested=Inf)</v>
+        <v>c(germination=0,leafDevelopment=0,tillering=0,stemElongation=0,booting=0,earing=0,anthesis=5,  grainFilling=-6,5, maturation=1.5, senescence=0, harvested=Inf)</v>
       </c>
       <c r="M96" s="56"/>
       <c r="N96" s="65" t="str">
@@ -7161,10 +7174,10 @@
       </c>
       <c r="P96" t="str">
         <f>"c(SOW=" &amp;P79&amp;", EMR="&amp;P80&amp;", EJU=4, TSI=NA, SIL=33.8,PM=4,MAT=Inf)"</f>
-        <v>c(SOW=3, EMR=8.5, EJU=4, TSI=NA, SIL=33.8,PM=4,MAT=Inf)</v>
-      </c>
-    </row>
-    <row r="97" spans="1:16">
+        <v>c(SOW=3, EMR=8,5, EJU=4, TSI=NA, SIL=33.8,PM=4,MAT=Inf)</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A97" s="59" t="s">
         <v>199</v>
       </c>
@@ -7199,7 +7212,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="98" spans="1:16">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A98" s="59" t="s">
         <v>200</v>
       </c>
@@ -7234,7 +7247,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="99" spans="1:16">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A99" s="60" t="s">
         <v>201</v>
       </c>
@@ -7269,7 +7282,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="100" spans="1:16">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A100" s="60" t="s">
         <v>202</v>
       </c>
@@ -7304,7 +7317,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="101" spans="1:16">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A101" s="61" t="s">
         <v>203</v>
       </c>
@@ -7313,23 +7326,23 @@
       </c>
       <c r="C101" s="54"/>
       <c r="D101" s="65" t="s">
-        <v>188</v>
+        <v>117</v>
       </c>
       <c r="E101" s="58"/>
-      <c r="F101" s="33" t="s">
-        <v>188</v>
+      <c r="F101" s="65" t="s">
+        <v>117</v>
       </c>
       <c r="G101" s="58"/>
-      <c r="H101" s="33" t="s">
-        <v>188</v>
+      <c r="H101" s="65" t="s">
+        <v>117</v>
       </c>
       <c r="I101" s="58"/>
       <c r="J101" s="33" t="s">
         <v>117</v>
       </c>
       <c r="K101" s="58"/>
-      <c r="L101" s="33" t="s">
-        <v>188</v>
+      <c r="L101" s="65" t="s">
+        <v>117</v>
       </c>
       <c r="M101" s="58"/>
       <c r="N101" s="65" t="s">
@@ -7339,7 +7352,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="102" spans="1:16">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A102" s="61" t="s">
         <v>204</v>
       </c>
@@ -7374,7 +7387,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="103" spans="1:16">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A103" s="59" t="s">
         <v>205</v>
       </c>
@@ -7406,10 +7419,10 @@
       </c>
       <c r="P103" t="str">
         <f>"is.after('SIL', "&amp;170/(P70-P69)&amp;")"</f>
-        <v>is.after('SIL', 6.53846153846154)</v>
-      </c>
-    </row>
-    <row r="104" spans="1:16">
+        <v>is.after('SIL', 6,53846153846154)</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A104" s="59" t="s">
         <v>206</v>
       </c>
@@ -7441,10 +7454,10 @@
       </c>
       <c r="P104" t="str">
         <f>"is.after('SIL', "&amp;170/(P70-P69)&amp;")"</f>
-        <v>is.after('SIL', 6.53846153846154)</v>
-      </c>
-    </row>
-    <row r="105" spans="1:16">
+        <v>is.after('SIL', 6,53846153846154)</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A105" s="59" t="s">
         <v>210</v>
       </c>
@@ -7478,7 +7491,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="106" spans="1:16">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A106" s="59" t="s">
         <v>212</v>
       </c>
@@ -7512,7 +7525,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="107" spans="1:16">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A107" s="59" t="s">
         <v>102</v>
       </c>
@@ -7546,7 +7559,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="108" spans="1:16">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A108" s="59" t="s">
         <v>103</v>
       </c>
@@ -7576,7 +7589,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="109" spans="1:16">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A109" s="59" t="s">
         <v>233</v>
       </c>
@@ -7604,10 +7617,10 @@
       </c>
       <c r="P109" t="str">
         <f>"is.after('SIL', "&amp;170/(P70-P69)&amp;")"</f>
-        <v>is.after('SIL', 6.53846153846154)</v>
-      </c>
-    </row>
-    <row r="110" spans="1:16">
+        <v>is.after('SIL', 6,53846153846154)</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A110" s="59" t="s">
         <v>104</v>
       </c>
@@ -7636,14 +7649,14 @@
       </c>
       <c r="N110" s="65" t="str">
         <f>"is.after('ANT', 5) &amp; is.before('ANT', "&amp; N85-1.5 &amp; ")"</f>
-        <v>is.after('ANT', 5) &amp; is.before('ANT', 41.5)</v>
+        <v>is.after('ANT', 5) &amp; is.before('ANT', 41,5)</v>
       </c>
       <c r="P110" t="str">
         <f>"is.after('SIL', "&amp;170/(P70-P69)&amp;") &amp; is.before('SIL', "&amp; 0.95*P81&amp;")"</f>
-        <v>is.after('SIL', 6.53846153846154) &amp; is.before('SIL', 32.11)</v>
-      </c>
-    </row>
-    <row r="111" spans="1:16">
+        <v>is.after('SIL', 6,53846153846154) &amp; is.before('SIL', 32,11)</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A111" s="61" t="s">
         <v>105</v>
       </c>
@@ -7668,14 +7681,14 @@
       </c>
       <c r="N111" s="65" t="str">
         <f>"is.after('EMR',  0) &amp; is.before('ANT', "&amp; N85-1.5 &amp; ")"</f>
-        <v>is.after('EMR',  0) &amp; is.before('ANT', 41.5)</v>
+        <v>is.after('EMR',  0) &amp; is.before('ANT', 41,5)</v>
       </c>
       <c r="P111" t="str">
         <f>"is.after('EMR',0) &amp; is.before('SIL', "&amp; 0.95*P81&amp;")"</f>
-        <v>is.after('EMR',0) &amp; is.before('SIL', 32.11)</v>
-      </c>
-    </row>
-    <row r="112" spans="1:16">
+        <v>is.after('EMR',0) &amp; is.before('SIL', 32,11)</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A112" s="62" t="s">
         <v>114</v>
       </c>
@@ -7702,10 +7715,10 @@
       </c>
       <c r="P112" t="str">
         <f>"is.after('EMR', 0) &amp; is.before('SIL', "&amp;170/(P70-P69)&amp;")"</f>
-        <v>is.after('EMR', 0) &amp; is.before('SIL', 6.53846153846154)</v>
-      </c>
-    </row>
-    <row r="113" spans="1:16">
+        <v>is.after('EMR', 0) &amp; is.before('SIL', 6,53846153846154)</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A113" s="64" t="s">
         <v>109</v>
       </c>
@@ -7727,7 +7740,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="114" spans="1:16">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A114" s="64" t="s">
         <v>110</v>
       </c>
@@ -7749,7 +7762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:16">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A115" s="64" t="s">
         <v>111</v>
       </c>
@@ -7771,7 +7784,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="116" spans="1:16">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A116" s="64" t="s">
         <v>112</v>
       </c>
@@ -7793,7 +7806,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="117" spans="1:16">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A117" s="64" t="s">
         <v>113</v>
       </c>
@@ -7815,7 +7828,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="118" spans="1:16">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>186</v>
       </c>
@@ -7841,7 +7854,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="119" spans="1:16">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A119" s="14" t="s">
         <v>219</v>
       </c>
@@ -7849,7 +7862,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="120" spans="1:16">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A120" s="14" t="s">
         <v>239</v>
       </c>
@@ -7870,11 +7883,11 @@
       </c>
       <c r="N120" t="str">
         <f>"is.before('ANT', "&amp; N85-1.5 &amp; ")"</f>
-        <v>is.before('ANT', 41.5)</v>
+        <v>is.before('ANT', 41,5)</v>
       </c>
       <c r="P120" t="str">
         <f>"is.before('SIL', "&amp; 0.95*P81&amp;")"</f>
-        <v>is.before('SIL', 32.11)</v>
+        <v>is.before('SIL', 32,11)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
deactivated photoperiod effect to test
</commit_message>
<xml_diff>
--- a/input/crops.xlsx
+++ b/input/crops.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA733C2-0B64-4B29-87F5-C112DCB5E8D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB0CAD2-B822-4453-8954-A967ED5C5826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1328,9 +1328,6 @@
     <t>0.002</t>
   </si>
   <si>
-    <t>0.17</t>
-  </si>
-  <si>
     <t>0.05</t>
   </si>
   <si>
@@ -1416,6 +1413,9 @@
   </si>
   <si>
     <t>is.before('R7',0)</t>
+  </si>
+  <si>
+    <t>0.017</t>
   </si>
 </sst>
 </file>
@@ -5017,11 +5017,11 @@
   <dimension ref="A1:P120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B91" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="E91" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D104" sqref="D104"/>
+      <selection pane="bottomRight" activeCell="N101" sqref="N101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6822,16 +6822,16 @@
         <v>3</v>
       </c>
       <c r="D77" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="F77" s="10">
+        <v>0</v>
+      </c>
+      <c r="H77" s="10">
+        <v>0</v>
+      </c>
+      <c r="J77" s="25" t="s">
         <v>266</v>
-      </c>
-      <c r="F77" s="10">
-        <v>0</v>
-      </c>
-      <c r="H77" s="10">
-        <v>0</v>
-      </c>
-      <c r="J77" s="25" t="s">
-        <v>267</v>
       </c>
       <c r="L77" s="10">
         <v>0</v>
@@ -6870,7 +6870,7 @@
         <v>4</v>
       </c>
       <c r="J79" s="25" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L79" s="10">
         <v>0</v>
@@ -6893,10 +6893,10 @@
         <v>5</v>
       </c>
       <c r="F80" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="H80" s="10" t="s">
         <v>269</v>
-      </c>
-      <c r="H80" s="10" t="s">
-        <v>270</v>
       </c>
       <c r="J80" s="25">
         <v>36</v>
@@ -6922,13 +6922,13 @@
         <v>8</v>
       </c>
       <c r="F81" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="H81" s="10" t="s">
         <v>271</v>
       </c>
-      <c r="H81" s="10" t="s">
+      <c r="J81" s="25" t="s">
         <v>272</v>
-      </c>
-      <c r="J81" s="25" t="s">
-        <v>273</v>
       </c>
       <c r="L81" s="10">
         <v>0</v>
@@ -6951,13 +6951,13 @@
         <v>6</v>
       </c>
       <c r="F82" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="H82" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="H82" s="10" t="s">
+      <c r="J82" s="25" t="s">
         <v>275</v>
-      </c>
-      <c r="J82" s="25" t="s">
-        <v>276</v>
       </c>
       <c r="L82" s="10">
         <v>0</v>
@@ -6977,10 +6977,10 @@
         <v>6</v>
       </c>
       <c r="F83" s="79" t="s">
+        <v>276</v>
+      </c>
+      <c r="H83" s="10" t="s">
         <v>277</v>
-      </c>
-      <c r="H83" s="10" t="s">
-        <v>278</v>
       </c>
       <c r="J83" s="25">
         <v>22</v>
@@ -7003,10 +7003,10 @@
         <v>15</v>
       </c>
       <c r="F84" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H84" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J84" s="25">
         <v>7</v>
@@ -7029,10 +7029,10 @@
         <v>43</v>
       </c>
       <c r="F85" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="H85" s="10" t="s">
         <v>279</v>
-      </c>
-      <c r="H85" s="10" t="s">
-        <v>280</v>
       </c>
       <c r="J85" s="6">
         <v>0</v>
@@ -7097,7 +7097,7 @@
         <v>0</v>
       </c>
       <c r="J88" s="28" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L88" s="55">
         <v>0</v>
@@ -7125,7 +7125,7 @@
         <v>0</v>
       </c>
       <c r="J89" s="28" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L89" s="55">
         <v>0</v>
@@ -7151,7 +7151,7 @@
         <v>0</v>
       </c>
       <c r="J90" s="29" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L90" s="55">
         <v>0</v>
@@ -7177,7 +7177,7 @@
         <v>0</v>
       </c>
       <c r="J91" s="29" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L91" s="55">
         <v>0</v>
@@ -7205,7 +7205,7 @@
         <v>0</v>
       </c>
       <c r="J92" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L92" s="55">
         <v>0</v>
@@ -7233,7 +7233,7 @@
         <v>0</v>
       </c>
       <c r="J93" s="28" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L93" s="55">
         <v>0</v>
@@ -7261,7 +7261,7 @@
         <v>0</v>
       </c>
       <c r="J94" s="28" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L94" s="55">
         <v>0</v>
@@ -7490,23 +7490,23 @@
       </c>
       <c r="C101" s="54"/>
       <c r="D101" s="65" t="s">
-        <v>117</v>
+        <v>188</v>
       </c>
       <c r="E101" s="58"/>
       <c r="F101" s="65" t="s">
-        <v>117</v>
+        <v>188</v>
       </c>
       <c r="G101" s="58"/>
       <c r="H101" s="65" t="s">
-        <v>117</v>
+        <v>188</v>
       </c>
       <c r="I101" s="58"/>
       <c r="J101" s="65" t="s">
-        <v>117</v>
+        <v>188</v>
       </c>
       <c r="K101" s="58"/>
       <c r="L101" s="65" t="s">
-        <v>117</v>
+        <v>188</v>
       </c>
       <c r="M101" s="58"/>
       <c r="N101" s="65" t="s">
@@ -7663,27 +7663,27 @@
         <v>208</v>
       </c>
       <c r="D106" s="65" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E106" s="14"/>
       <c r="F106" s="65" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G106" s="14"/>
       <c r="H106" s="65" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I106" s="14"/>
       <c r="J106" s="65" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K106" s="14"/>
       <c r="L106" s="65" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="M106" s="14"/>
       <c r="N106" s="65" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="P106" s="65" t="s">
         <v>117</v>
@@ -7697,15 +7697,15 @@
         <v>208</v>
       </c>
       <c r="D107" s="65" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E107" s="14"/>
       <c r="F107" s="33" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G107" s="57"/>
       <c r="H107" s="33" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I107" s="57"/>
       <c r="J107" s="33" t="s">
@@ -7713,11 +7713,11 @@
       </c>
       <c r="K107" s="57"/>
       <c r="L107" s="33" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="M107" s="57"/>
       <c r="N107" s="65" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="P107" t="s">
         <v>195</v>
@@ -7732,19 +7732,19 @@
       </c>
       <c r="C108" s="54"/>
       <c r="D108" s="65" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F108" s="65" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H108" s="33" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J108" s="33" t="s">
         <v>211</v>
       </c>
       <c r="L108" s="65" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="N108" s="65" t="s">
         <v>190</v>
@@ -7805,7 +7805,7 @@
         <v>is.after('grainFilling', 0) &amp; is.before('maturation',0)</v>
       </c>
       <c r="J110" s="33" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L110" s="33" t="str">
         <f>"is.after('grainFilling', 0) &amp; is.before('maturation',0)"</f>
@@ -7829,19 +7829,19 @@
       </c>
       <c r="C111" s="54"/>
       <c r="D111" s="65" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F111" s="65" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H111" s="65" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J111" s="33" t="s">
         <v>210</v>
       </c>
       <c r="L111" s="65" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="N111" s="65" t="str">
         <f>"is.after('EMR',  0) &amp; is.before('ANT', "&amp; N85-1.5 &amp; ")"</f>
@@ -7863,16 +7863,16 @@
         <v>230</v>
       </c>
       <c r="F112" s="65" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H112" s="65" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J112" s="33" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L112" s="65" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N112" s="65" t="s">
         <v>191</v>
@@ -8031,19 +8031,19 @@
         <v>231</v>
       </c>
       <c r="D120" t="s">
+        <v>293</v>
+      </c>
+      <c r="F120" t="s">
+        <v>293</v>
+      </c>
+      <c r="H120" t="s">
+        <v>293</v>
+      </c>
+      <c r="J120" t="s">
         <v>294</v>
       </c>
-      <c r="F120" t="s">
-        <v>294</v>
-      </c>
-      <c r="H120" t="s">
-        <v>294</v>
-      </c>
-      <c r="J120" t="s">
-        <v>295</v>
-      </c>
       <c r="L120" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="N120" t="str">
         <f>"is.before('ANT', "&amp; N85-1.5 &amp; ")"</f>

</xml_diff>

<commit_message>
fixed a filter for chickpea
</commit_message>
<xml_diff>
--- a/input/crops.xlsx
+++ b/input/crops.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB0CAD2-B822-4453-8954-A967ED5C5826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB30AB07-949B-44AC-8F8F-A047F658F632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5017,11 +5017,11 @@
   <dimension ref="A1:P120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="E91" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="E100" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="N101" sqref="N101"/>
+      <selection pane="bottomRight" activeCell="J101" sqref="J101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7502,7 +7502,7 @@
       </c>
       <c r="I101" s="58"/>
       <c r="J101" s="65" t="s">
-        <v>188</v>
+        <v>117</v>
       </c>
       <c r="K101" s="58"/>
       <c r="L101" s="65" t="s">

</xml_diff>

<commit_message>
Fixed computation of cFTSWrootZone
</commit_message>
<xml_diff>
--- a/input/crops.xlsx
+++ b/input/crops.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB30AB07-949B-44AC-8F8F-A047F658F632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52911013-C408-4BD8-96A7-05D3B65F2730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -528,7 +528,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="297">
   <si>
     <t>CROP:</t>
   </si>
@@ -1415,7 +1415,10 @@
     <t>is.before('R7',0)</t>
   </si>
   <si>
-    <t>0.017</t>
+    <t>is.after('leafDevelopment', 0) &amp; is.before('stemElongation',0)</t>
+  </si>
+  <si>
+    <t>0.17</t>
   </si>
 </sst>
 </file>
@@ -5017,11 +5020,11 @@
   <dimension ref="A1:P120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="E100" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B85" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="J101" sqref="J101"/>
+      <selection pane="bottomRight" activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6822,7 +6825,7 @@
         <v>3</v>
       </c>
       <c r="D77" s="10" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="F77" s="10">
         <v>0</v>
@@ -7490,7 +7493,7 @@
       </c>
       <c r="C101" s="54"/>
       <c r="D101" s="65" t="s">
-        <v>188</v>
+        <v>295</v>
       </c>
       <c r="E101" s="58"/>
       <c r="F101" s="65" t="s">
@@ -7525,7 +7528,7 @@
       </c>
       <c r="C102" s="54"/>
       <c r="D102" s="65" t="s">
-        <v>188</v>
+        <v>295</v>
       </c>
       <c r="E102" s="58"/>
       <c r="F102" s="33" t="s">

</xml_diff>